<commit_message>
add color format and refactor
Add new Excel processing script with conditional formatting and output files
</commit_message>
<xml_diff>
--- a/data_transformation/excel_files/optimized_excel_with_regx.xlsx
+++ b/data_transformation/excel_files/optimized_excel_with_regx.xlsx
@@ -182,7 +182,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -1125,6 +1140,1006 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="greaterThan">
+      <formula>$C10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
+      <formula>$C11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="greaterThan">
+      <formula>$C12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="greaterThan">
+      <formula>$C13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="cellIs" dxfId="0" priority="23" operator="greaterThan">
+      <formula>$C14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="greaterThan">
+      <formula>$C15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="greaterThan">
+      <formula>$C16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="greaterThan">
+      <formula>$C17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="cellIs" dxfId="0" priority="31" operator="greaterThan">
+      <formula>$C18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="cellIs" dxfId="0" priority="33" operator="greaterThan">
+      <formula>$C19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="cellIs" dxfId="0" priority="35" operator="greaterThan">
+      <formula>$C20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="greaterThan">
+      <formula>$C21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="cellIs" dxfId="0" priority="39" operator="greaterThan">
+      <formula>$C22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="cellIs" dxfId="0" priority="41" operator="greaterThan">
+      <formula>$C23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="cellIs" dxfId="0" priority="43" operator="greaterThan">
+      <formula>$C24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="cellIs" dxfId="0" priority="45" operator="greaterThan">
+      <formula>$C25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="cellIs" dxfId="0" priority="47" operator="greaterThan">
+      <formula>$C26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="cellIs" dxfId="0" priority="49" operator="greaterThan">
+      <formula>$C27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$C3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>$C4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
+      <formula>$C5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
+      <formula>$C6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
+      <formula>$C7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="greaterThan">
+      <formula>$C8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
+      <formula>$C9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="1" priority="16" operator="greaterThan">
+      <formula>$B10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="1" priority="18" operator="greaterThan">
+      <formula>$B11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="1" priority="20" operator="greaterThan">
+      <formula>$B12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="1" priority="22" operator="greaterThan">
+      <formula>$B13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="1" priority="24" operator="greaterThan">
+      <formula>$B14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="greaterThan">
+      <formula>$B15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="cellIs" dxfId="1" priority="28" operator="greaterThan">
+      <formula>$B16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="cellIs" dxfId="1" priority="30" operator="greaterThan">
+      <formula>$B17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="cellIs" dxfId="1" priority="32" operator="greaterThan">
+      <formula>$B18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="cellIs" dxfId="1" priority="34" operator="greaterThan">
+      <formula>$B19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="cellIs" dxfId="1" priority="36" operator="greaterThan">
+      <formula>$B20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="1" priority="38" operator="greaterThan">
+      <formula>$B21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="1" priority="40" operator="greaterThan">
+      <formula>$B22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="cellIs" dxfId="1" priority="42" operator="greaterThan">
+      <formula>$B23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="1" priority="44" operator="greaterThan">
+      <formula>$B24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="cellIs" dxfId="1" priority="46" operator="greaterThan">
+      <formula>$B25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="cellIs" dxfId="1" priority="48" operator="greaterThan">
+      <formula>$B26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="1" priority="50" operator="greaterThan">
+      <formula>$B27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>$B3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+      <formula>$B4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThan">
+      <formula>$B5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThan">
+      <formula>$B6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="greaterThan">
+      <formula>$B7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="greaterThan">
+      <formula>$B8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThan">
+      <formula>$B9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="0" priority="65" operator="greaterThan">
+      <formula>$E10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="0" priority="67" operator="greaterThan">
+      <formula>$E11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="0" priority="69" operator="greaterThan">
+      <formula>$E12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="0" priority="71" operator="greaterThan">
+      <formula>$E13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="0" priority="73" operator="greaterThan">
+      <formula>$E14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="0" priority="75" operator="greaterThan">
+      <formula>$E15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="cellIs" dxfId="0" priority="77" operator="greaterThan">
+      <formula>$E16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="cellIs" dxfId="0" priority="79" operator="greaterThan">
+      <formula>$E17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="cellIs" dxfId="0" priority="81" operator="greaterThan">
+      <formula>$E18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="0" priority="83" operator="greaterThan">
+      <formula>$E19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="cellIs" dxfId="0" priority="85" operator="greaterThan">
+      <formula>$E20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="cellIs" dxfId="0" priority="87" operator="greaterThan">
+      <formula>$E21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="cellIs" dxfId="0" priority="89" operator="greaterThan">
+      <formula>$E22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="cellIs" dxfId="0" priority="91" operator="greaterThan">
+      <formula>$E23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="0" priority="93" operator="greaterThan">
+      <formula>$E24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="cellIs" dxfId="0" priority="95" operator="greaterThan">
+      <formula>$E25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="cellIs" dxfId="0" priority="97" operator="greaterThan">
+      <formula>$E26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="0" priority="99" operator="greaterThan">
+      <formula>$E27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="0" priority="51" operator="greaterThan">
+      <formula>$E3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="greaterThan">
+      <formula>$E4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="0" priority="55" operator="greaterThan">
+      <formula>$E5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="0" priority="57" operator="greaterThan">
+      <formula>$E6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="0" priority="59" operator="greaterThan">
+      <formula>$E7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="0" priority="61" operator="greaterThan">
+      <formula>$E8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="0" priority="63" operator="greaterThan">
+      <formula>$E9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="1" priority="66" operator="greaterThan">
+      <formula>$D10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="1" priority="68" operator="greaterThan">
+      <formula>$D11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="1" priority="70" operator="greaterThan">
+      <formula>$D12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="1" priority="72" operator="greaterThan">
+      <formula>$D13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="1" priority="74" operator="greaterThan">
+      <formula>$D14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="1" priority="76" operator="greaterThan">
+      <formula>$D15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="1" priority="78" operator="greaterThan">
+      <formula>$D16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="cellIs" dxfId="1" priority="80" operator="greaterThan">
+      <formula>$D17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="1" priority="82" operator="greaterThan">
+      <formula>$D18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="1" priority="84" operator="greaterThan">
+      <formula>$D19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="1" priority="86" operator="greaterThan">
+      <formula>$D20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="1" priority="88" operator="greaterThan">
+      <formula>$D21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="1" priority="90" operator="greaterThan">
+      <formula>$D22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="1" priority="92" operator="greaterThan">
+      <formula>$D23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="1" priority="94" operator="greaterThan">
+      <formula>$D24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="1" priority="96" operator="greaterThan">
+      <formula>$D25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="1" priority="98" operator="greaterThan">
+      <formula>$D26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="1" priority="100" operator="greaterThan">
+      <formula>$D27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="1" priority="52" operator="greaterThan">
+      <formula>$D3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="1" priority="54" operator="greaterThan">
+      <formula>$D4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="1" priority="56" operator="greaterThan">
+      <formula>$D5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="1" priority="58" operator="greaterThan">
+      <formula>$D6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="1" priority="60" operator="greaterThan">
+      <formula>$D7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="1" priority="62" operator="greaterThan">
+      <formula>$D8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="1" priority="64" operator="greaterThan">
+      <formula>$D9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="cellIs" dxfId="0" priority="115" operator="greaterThan">
+      <formula>$G10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="cellIs" dxfId="0" priority="117" operator="greaterThan">
+      <formula>$G11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="cellIs" dxfId="0" priority="119" operator="greaterThan">
+      <formula>$G12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="0" priority="121" operator="greaterThan">
+      <formula>$G13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="cellIs" dxfId="0" priority="123" operator="greaterThan">
+      <formula>$G14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="cellIs" dxfId="0" priority="125" operator="greaterThan">
+      <formula>$G15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="cellIs" dxfId="0" priority="127" operator="greaterThan">
+      <formula>$G16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="cellIs" dxfId="0" priority="129" operator="greaterThan">
+      <formula>$G17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="0" priority="131" operator="greaterThan">
+      <formula>$G18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="cellIs" dxfId="0" priority="133" operator="greaterThan">
+      <formula>$G19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="0" priority="135" operator="greaterThan">
+      <formula>$G20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="cellIs" dxfId="0" priority="137" operator="greaterThan">
+      <formula>$G21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="0" priority="139" operator="greaterThan">
+      <formula>$G22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="cellIs" dxfId="0" priority="141" operator="greaterThan">
+      <formula>$G23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="cellIs" dxfId="0" priority="143" operator="greaterThan">
+      <formula>$G24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="0" priority="145" operator="greaterThan">
+      <formula>$G25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="cellIs" dxfId="0" priority="147" operator="greaterThan">
+      <formula>$G26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="0" priority="149" operator="greaterThan">
+      <formula>$G27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="0" priority="101" operator="greaterThan">
+      <formula>$G3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="cellIs" dxfId="0" priority="103" operator="greaterThan">
+      <formula>$G4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="0" priority="105" operator="greaterThan">
+      <formula>$G5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="0" priority="107" operator="greaterThan">
+      <formula>$G6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="0" priority="109" operator="greaterThan">
+      <formula>$G7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="0" priority="111" operator="greaterThan">
+      <formula>$G8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="0" priority="113" operator="greaterThan">
+      <formula>$G9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="1" priority="116" operator="greaterThan">
+      <formula>$F10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="1" priority="118" operator="greaterThan">
+      <formula>$F11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="1" priority="120" operator="greaterThan">
+      <formula>$F12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" dxfId="1" priority="122" operator="greaterThan">
+      <formula>$F13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="1" priority="124" operator="greaterThan">
+      <formula>$F14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" dxfId="1" priority="126" operator="greaterThan">
+      <formula>$F15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="cellIs" dxfId="1" priority="128" operator="greaterThan">
+      <formula>$F16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" dxfId="1" priority="130" operator="greaterThan">
+      <formula>$F17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="1" priority="132" operator="greaterThan">
+      <formula>$F18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="cellIs" dxfId="1" priority="134" operator="greaterThan">
+      <formula>$F19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" dxfId="1" priority="136" operator="greaterThan">
+      <formula>$F20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
+    <cfRule type="cellIs" dxfId="1" priority="138" operator="greaterThan">
+      <formula>$F21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="cellIs" dxfId="1" priority="140" operator="greaterThan">
+      <formula>$F22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="cellIs" dxfId="1" priority="142" operator="greaterThan">
+      <formula>$F23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="cellIs" dxfId="1" priority="144" operator="greaterThan">
+      <formula>$F24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25">
+    <cfRule type="cellIs" dxfId="1" priority="146" operator="greaterThan">
+      <formula>$F25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26">
+    <cfRule type="cellIs" dxfId="1" priority="148" operator="greaterThan">
+      <formula>$F26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27">
+    <cfRule type="cellIs" dxfId="1" priority="150" operator="greaterThan">
+      <formula>$F27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="1" priority="102" operator="greaterThan">
+      <formula>$F3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="cellIs" dxfId="1" priority="104" operator="greaterThan">
+      <formula>$F4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="1" priority="106" operator="greaterThan">
+      <formula>$F5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="1" priority="108" operator="greaterThan">
+      <formula>$F6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="1" priority="110" operator="greaterThan">
+      <formula>$F7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="1" priority="112" operator="greaterThan">
+      <formula>$F8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" dxfId="1" priority="114" operator="greaterThan">
+      <formula>$F9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="cellIs" dxfId="0" priority="165" operator="greaterThan">
+      <formula>$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="0" priority="167" operator="greaterThan">
+      <formula>$I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" dxfId="0" priority="169" operator="greaterThan">
+      <formula>$I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="cellIs" dxfId="0" priority="171" operator="greaterThan">
+      <formula>$I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="cellIs" dxfId="0" priority="173" operator="greaterThan">
+      <formula>$I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="0" priority="175" operator="greaterThan">
+      <formula>$I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="cellIs" dxfId="0" priority="177" operator="greaterThan">
+      <formula>$I16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="cellIs" dxfId="0" priority="179" operator="greaterThan">
+      <formula>$I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="cellIs" dxfId="0" priority="181" operator="greaterThan">
+      <formula>$I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" dxfId="0" priority="183" operator="greaterThan">
+      <formula>$I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" dxfId="0" priority="185" operator="greaterThan">
+      <formula>$I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="cellIs" dxfId="0" priority="187" operator="greaterThan">
+      <formula>$I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" dxfId="0" priority="189" operator="greaterThan">
+      <formula>$I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="0" priority="191" operator="greaterThan">
+      <formula>$I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="0" priority="193" operator="greaterThan">
+      <formula>$I24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="cellIs" dxfId="0" priority="195" operator="greaterThan">
+      <formula>$I25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="0" priority="197" operator="greaterThan">
+      <formula>$I26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="cellIs" dxfId="0" priority="199" operator="greaterThan">
+      <formula>$I27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="cellIs" dxfId="0" priority="151" operator="greaterThan">
+      <formula>$I3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="cellIs" dxfId="0" priority="153" operator="greaterThan">
+      <formula>$I4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="0" priority="155" operator="greaterThan">
+      <formula>$I5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="0" priority="157" operator="greaterThan">
+      <formula>$I6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="0" priority="159" operator="greaterThan">
+      <formula>$I7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" dxfId="0" priority="161" operator="greaterThan">
+      <formula>$I8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="0" priority="163" operator="greaterThan">
+      <formula>$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="cellIs" dxfId="1" priority="166" operator="greaterThan">
+      <formula>$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="1" priority="168" operator="greaterThan">
+      <formula>$H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="1" priority="170" operator="greaterThan">
+      <formula>$H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="1" priority="172" operator="greaterThan">
+      <formula>$H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="1" priority="174" operator="greaterThan">
+      <formula>$H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="1" priority="176" operator="greaterThan">
+      <formula>$H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="1" priority="178" operator="greaterThan">
+      <formula>$H16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="1" priority="180" operator="greaterThan">
+      <formula>$H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="1" priority="182" operator="greaterThan">
+      <formula>$H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="cellIs" dxfId="1" priority="184" operator="greaterThan">
+      <formula>$H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" dxfId="1" priority="186" operator="greaterThan">
+      <formula>$H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="cellIs" dxfId="1" priority="188" operator="greaterThan">
+      <formula>$H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="cellIs" dxfId="1" priority="190" operator="greaterThan">
+      <formula>$H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" dxfId="1" priority="192" operator="greaterThan">
+      <formula>$H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="1" priority="194" operator="greaterThan">
+      <formula>$H24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" dxfId="1" priority="196" operator="greaterThan">
+      <formula>$H25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="1" priority="198" operator="greaterThan">
+      <formula>$H26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="cellIs" dxfId="1" priority="200" operator="greaterThan">
+      <formula>$H27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="cellIs" dxfId="1" priority="152" operator="greaterThan">
+      <formula>$H3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="cellIs" dxfId="1" priority="154" operator="greaterThan">
+      <formula>$H4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="1" priority="156" operator="greaterThan">
+      <formula>$H5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="cellIs" dxfId="1" priority="158" operator="greaterThan">
+      <formula>$H6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" dxfId="1" priority="160" operator="greaterThan">
+      <formula>$H7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="cellIs" dxfId="1" priority="162" operator="greaterThan">
+      <formula>$H8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="cellIs" dxfId="1" priority="164" operator="greaterThan">
+      <formula>$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>